<commit_message>
Even more species with no maps
</commit_message>
<xml_diff>
--- a/systematic lit review progress notes.xlsx
+++ b/systematic lit review progress notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherineschluth/bansallab/humanhelminths/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F1137CC-7F4F-4141-81D8-A7C2BED3D108}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{03F621CA-3AD2-E746-A366-4D3F1C990B48}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1103,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2055,7 +2055,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>47</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>97</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>189</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>45</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>41</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>65</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>219</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>228</v>
       </c>
@@ -2167,13 +2167,20 @@
       <c r="C72" t="s">
         <v>4</v>
       </c>
-      <c r="D72" s="2"/>
-      <c r="E72" s="2"/>
+      <c r="D72" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E72" s="2">
+        <v>43411</v>
+      </c>
       <c r="F72">
         <v>7</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>172</v>
       </c>
@@ -2183,13 +2190,20 @@
       <c r="C73" t="s">
         <v>4</v>
       </c>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
+      <c r="D73" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E73" s="2">
+        <v>43411</v>
+      </c>
       <c r="F73">
         <v>6</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>42</v>
       </c>
@@ -2199,11 +2213,20 @@
       <c r="C74" t="s">
         <v>4</v>
       </c>
+      <c r="D74" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E74" s="2">
+        <v>43411</v>
+      </c>
       <c r="F74">
         <v>6</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>84</v>
       </c>
@@ -2213,11 +2236,20 @@
       <c r="C75" t="s">
         <v>4</v>
       </c>
+      <c r="D75" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E75" s="2">
+        <v>43411</v>
+      </c>
       <c r="F75">
         <v>6</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>37</v>
       </c>
@@ -2227,11 +2259,20 @@
       <c r="C76" t="s">
         <v>4</v>
       </c>
+      <c r="D76" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E76" s="2">
+        <v>43411</v>
+      </c>
       <c r="F76">
         <v>6</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>30</v>
       </c>
@@ -2241,11 +2282,20 @@
       <c r="C77" t="s">
         <v>4</v>
       </c>
+      <c r="D77" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E77" s="2">
+        <v>43411</v>
+      </c>
       <c r="F77">
         <v>6</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>98</v>
       </c>
@@ -2255,11 +2305,20 @@
       <c r="C78" t="s">
         <v>4</v>
       </c>
+      <c r="D78" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E78" s="2">
+        <v>43411</v>
+      </c>
       <c r="F78">
         <v>6</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>109</v>
       </c>
@@ -2269,12 +2328,20 @@
       <c r="C79" t="s">
         <v>4</v>
       </c>
-      <c r="D79" s="2"/>
+      <c r="D79" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E79" s="2">
+        <v>43411</v>
+      </c>
       <c r="F79">
         <v>6</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>190</v>
       </c>
@@ -2284,13 +2351,20 @@
       <c r="C80" t="s">
         <v>4</v>
       </c>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
+      <c r="D80" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E80" s="2">
+        <v>43411</v>
+      </c>
       <c r="F80">
         <v>6</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>165</v>
       </c>
@@ -2300,13 +2374,20 @@
       <c r="C81" t="s">
         <v>4</v>
       </c>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2"/>
+      <c r="D81" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E81" s="2">
+        <v>43411</v>
+      </c>
       <c r="F81">
         <v>6</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>112</v>
       </c>
@@ -2316,12 +2397,20 @@
       <c r="C82" t="s">
         <v>4</v>
       </c>
-      <c r="D82" s="2"/>
+      <c r="D82" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E82" s="2">
+        <v>43411</v>
+      </c>
       <c r="F82">
         <v>6</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>58</v>
       </c>
@@ -2331,11 +2420,20 @@
       <c r="C83" t="s">
         <v>4</v>
       </c>
+      <c r="D83" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E83" s="2">
+        <v>43411</v>
+      </c>
       <c r="F83">
         <v>5</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>140</v>
       </c>
@@ -2345,12 +2443,20 @@
       <c r="C84" t="s">
         <v>4</v>
       </c>
-      <c r="D84" s="2"/>
+      <c r="D84" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E84" s="2">
+        <v>43411</v>
+      </c>
       <c r="F84">
         <v>5</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>191</v>
       </c>
@@ -2360,13 +2466,20 @@
       <c r="C85" t="s">
         <v>4</v>
       </c>
-      <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
+      <c r="D85" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E85" s="2">
+        <v>43411</v>
+      </c>
       <c r="F85">
         <v>5</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>146</v>
       </c>
@@ -2376,12 +2489,20 @@
       <c r="C86" t="s">
         <v>4</v>
       </c>
-      <c r="D86" s="2"/>
+      <c r="D86" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E86" s="2">
+        <v>43411</v>
+      </c>
       <c r="F86">
         <v>5</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>232</v>
       </c>
@@ -2391,13 +2512,20 @@
       <c r="C87" t="s">
         <v>4</v>
       </c>
-      <c r="D87" s="2"/>
-      <c r="E87" s="2"/>
+      <c r="D87" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E87" s="2">
+        <v>43411</v>
+      </c>
       <c r="F87">
         <v>5</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>44</v>
       </c>
@@ -2407,11 +2535,20 @@
       <c r="C88" t="s">
         <v>4</v>
       </c>
+      <c r="D88" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E88" s="2">
+        <v>43411</v>
+      </c>
       <c r="F88">
         <v>4</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>116</v>
       </c>
@@ -2421,12 +2558,20 @@
       <c r="C89" t="s">
         <v>4</v>
       </c>
-      <c r="D89" s="2"/>
+      <c r="D89" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E89" s="2">
+        <v>43411</v>
+      </c>
       <c r="F89">
         <v>4</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>223</v>
       </c>
@@ -2436,13 +2581,20 @@
       <c r="C90" t="s">
         <v>4</v>
       </c>
-      <c r="D90" s="2"/>
-      <c r="E90" s="2"/>
+      <c r="D90" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E90" s="2">
+        <v>43411</v>
+      </c>
       <c r="F90">
         <v>4</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>96</v>
       </c>
@@ -2452,11 +2604,20 @@
       <c r="C91" t="s">
         <v>4</v>
       </c>
+      <c r="D91" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E91" s="2">
+        <v>43411</v>
+      </c>
       <c r="F91">
         <v>4</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>208</v>
       </c>
@@ -2466,13 +2627,20 @@
       <c r="C92" t="s">
         <v>4</v>
       </c>
-      <c r="D92" s="2"/>
-      <c r="E92" s="2"/>
+      <c r="D92" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E92" s="2">
+        <v>43411</v>
+      </c>
       <c r="F92">
         <v>4</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>133</v>
       </c>
@@ -2482,12 +2650,20 @@
       <c r="C93" t="s">
         <v>4</v>
       </c>
-      <c r="D93" s="2"/>
+      <c r="D93" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E93" s="2">
+        <v>43411</v>
+      </c>
       <c r="F93">
         <v>4</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>99</v>
       </c>
@@ -2497,12 +2673,20 @@
       <c r="C94" t="s">
         <v>4</v>
       </c>
-      <c r="D94" s="2"/>
+      <c r="D94" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E94" s="2">
+        <v>43411</v>
+      </c>
       <c r="F94">
         <v>4</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>90</v>
       </c>
@@ -2512,11 +2696,20 @@
       <c r="C95" t="s">
         <v>4</v>
       </c>
+      <c r="D95" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E95" s="2">
+        <v>43411</v>
+      </c>
       <c r="F95">
         <v>4</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>166</v>
       </c>
@@ -2526,10 +2719,17 @@
       <c r="C96" t="s">
         <v>4</v>
       </c>
-      <c r="D96" s="2"/>
-      <c r="E96" s="2"/>
+      <c r="D96" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E96" s="2">
+        <v>43411</v>
+      </c>
       <c r="F96">
         <v>4</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
@@ -2542,8 +2742,17 @@
       <c r="C97" t="s">
         <v>4</v>
       </c>
+      <c r="D97" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E97" s="2">
+        <v>43411</v>
+      </c>
       <c r="F97">
         <v>4</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
@@ -2556,8 +2765,17 @@
       <c r="C98" t="s">
         <v>4</v>
       </c>
+      <c r="D98" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E98" s="2">
+        <v>43411</v>
+      </c>
       <c r="F98">
         <v>4</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
@@ -2570,9 +2788,17 @@
       <c r="C99" t="s">
         <v>4</v>
       </c>
-      <c r="D99" s="2"/>
+      <c r="D99" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E99" s="2">
+        <v>43411</v>
+      </c>
       <c r="F99">
         <v>3</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
@@ -2585,8 +2811,17 @@
       <c r="C100" t="s">
         <v>4</v>
       </c>
+      <c r="D100" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E100" s="2">
+        <v>43411</v>
+      </c>
       <c r="F100">
         <v>3</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
@@ -2599,8 +2834,17 @@
       <c r="C101" t="s">
         <v>4</v>
       </c>
+      <c r="D101" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E101" s="2">
+        <v>43411</v>
+      </c>
       <c r="F101">
         <v>3</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
@@ -2613,10 +2857,17 @@
       <c r="C102" t="s">
         <v>4</v>
       </c>
-      <c r="D102" s="2"/>
-      <c r="E102" s="2"/>
+      <c r="D102" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E102" s="2">
+        <v>43411</v>
+      </c>
       <c r="F102">
         <v>3</v>
+      </c>
+      <c r="G102">
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
@@ -2629,9 +2880,17 @@
       <c r="C103" t="s">
         <v>4</v>
       </c>
-      <c r="D103" s="2"/>
+      <c r="D103" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E103" s="2">
+        <v>43411</v>
+      </c>
       <c r="F103">
         <v>3</v>
+      </c>
+      <c r="G103">
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
@@ -2644,9 +2903,17 @@
       <c r="C104" t="s">
         <v>4</v>
       </c>
-      <c r="D104" s="2"/>
+      <c r="D104" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E104" s="2">
+        <v>43411</v>
+      </c>
       <c r="F104">
         <v>3</v>
+      </c>
+      <c r="G104">
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
@@ -2659,9 +2926,17 @@
       <c r="C105" t="s">
         <v>4</v>
       </c>
-      <c r="D105" s="2"/>
+      <c r="D105" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E105" s="2">
+        <v>43411</v>
+      </c>
       <c r="F105">
         <v>3</v>
+      </c>
+      <c r="G105">
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
@@ -2674,10 +2949,17 @@
       <c r="C106" t="s">
         <v>4</v>
       </c>
-      <c r="D106" s="2"/>
-      <c r="E106" s="2"/>
+      <c r="D106" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E106" s="2">
+        <v>43411</v>
+      </c>
       <c r="F106">
         <v>3</v>
+      </c>
+      <c r="G106">
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
@@ -2690,10 +2972,17 @@
       <c r="C107" t="s">
         <v>4</v>
       </c>
-      <c r="D107" s="2"/>
-      <c r="E107" s="2"/>
+      <c r="D107" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E107" s="2">
+        <v>43411</v>
+      </c>
       <c r="F107">
         <v>3</v>
+      </c>
+      <c r="G107">
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
@@ -2706,10 +2995,17 @@
       <c r="C108" t="s">
         <v>4</v>
       </c>
-      <c r="D108" s="2"/>
-      <c r="E108" s="2"/>
+      <c r="D108" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E108" s="2">
+        <v>43411</v>
+      </c>
       <c r="F108">
         <v>3</v>
+      </c>
+      <c r="G108">
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
@@ -2722,9 +3018,17 @@
       <c r="C109" t="s">
         <v>4</v>
       </c>
-      <c r="D109" s="2"/>
+      <c r="D109" s="2">
+        <v>43410</v>
+      </c>
+      <c r="E109" s="2">
+        <v>43411</v>
+      </c>
       <c r="F109">
         <v>2</v>
+      </c>
+      <c r="G109">
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Lots of accidental schisto results, very little of pretty much anything else
</commit_message>
<xml_diff>
--- a/systematic lit review progress notes.xlsx
+++ b/systematic lit review progress notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherineschluth/bansallab/humanhelminths/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03F621CA-3AD2-E746-A366-4D3F1C990B48}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D7E2777-B805-B445-88F8-95763E7FFC0C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1103,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1150,8 +1150,14 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
+      <c r="D2" s="2">
+        <v>43417</v>
+      </c>
       <c r="F2">
         <v>2319</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1178,8 +1184,14 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
+      <c r="D4" s="2">
+        <v>43417</v>
+      </c>
       <c r="F4">
         <v>948</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1192,8 +1204,14 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
+      <c r="D5" s="2">
+        <v>43417</v>
+      </c>
       <c r="F5">
         <v>705</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1220,8 +1238,14 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
+      <c r="D7" s="2">
+        <v>43417</v>
+      </c>
       <c r="F7">
         <v>654</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1262,8 +1286,14 @@
       <c r="C10" t="s">
         <v>4</v>
       </c>
+      <c r="D10" s="2">
+        <v>43417</v>
+      </c>
       <c r="F10">
         <v>409</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1304,8 +1334,14 @@
       <c r="C13" t="s">
         <v>4</v>
       </c>
+      <c r="D13" s="2">
+        <v>43417</v>
+      </c>
       <c r="F13">
         <v>320</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1350,7 +1386,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1364,7 +1400,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1378,7 +1414,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1392,7 +1428,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -1406,7 +1442,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1420,7 +1456,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1434,7 +1470,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -1448,7 +1484,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>102</v>
       </c>
@@ -1463,7 +1499,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>114</v>
       </c>
@@ -1478,7 +1514,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -1488,11 +1524,17 @@
       <c r="C26" t="s">
         <v>4</v>
       </c>
+      <c r="D26" s="2">
+        <v>43417</v>
+      </c>
       <c r="F26">
         <v>99</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>101</v>
       </c>
@@ -1507,7 +1549,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -1521,7 +1563,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -1535,7 +1577,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1549,7 +1591,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>168</v>
       </c>
@@ -1564,7 +1606,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>25</v>
       </c>
@@ -1644,8 +1686,14 @@
       <c r="C37" t="s">
         <v>4</v>
       </c>
+      <c r="D37" s="2">
+        <v>43417</v>
+      </c>
       <c r="F37">
         <v>37</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1686,9 +1734,14 @@
       <c r="C40" t="s">
         <v>4</v>
       </c>
-      <c r="D40" s="2"/>
+      <c r="D40" s="2">
+        <v>43417</v>
+      </c>
       <c r="F40">
         <v>35</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -1724,8 +1777,14 @@
       <c r="C42" t="s">
         <v>4</v>
       </c>
+      <c r="D42" s="2">
+        <v>43417</v>
+      </c>
       <c r="F42">
         <v>34</v>
+      </c>
+      <c r="G42">
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -1738,8 +1797,14 @@
       <c r="C43" t="s">
         <v>4</v>
       </c>
+      <c r="D43" s="2">
+        <v>43417</v>
+      </c>
       <c r="F43">
         <v>32</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -1816,7 +1881,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>69</v>
       </c>
@@ -1830,7 +1895,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>111</v>
       </c>
@@ -1845,7 +1910,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>125</v>
       </c>
@@ -1860,7 +1925,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -1874,7 +1939,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>167</v>
       </c>
@@ -1889,7 +1954,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>103</v>
       </c>
@@ -1899,12 +1964,20 @@
       <c r="C54" t="s">
         <v>4</v>
       </c>
-      <c r="D54" s="2"/>
+      <c r="D54" s="2">
+        <v>43417</v>
+      </c>
+      <c r="E54" s="2">
+        <v>43417</v>
+      </c>
       <c r="F54">
         <v>17</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>158</v>
       </c>
@@ -1914,13 +1987,20 @@
       <c r="C55" t="s">
         <v>4</v>
       </c>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
+      <c r="D55" s="2">
+        <v>43417</v>
+      </c>
+      <c r="E55" s="2">
+        <v>43417</v>
+      </c>
       <c r="F55">
         <v>17</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>196</v>
       </c>
@@ -1930,13 +2010,20 @@
       <c r="C56" t="s">
         <v>4</v>
       </c>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
+      <c r="D56" s="2">
+        <v>43417</v>
+      </c>
+      <c r="E56" s="2">
+        <v>43417</v>
+      </c>
       <c r="F56">
         <v>17</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>202</v>
       </c>
@@ -1946,13 +2033,20 @@
       <c r="C57" t="s">
         <v>4</v>
       </c>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
+      <c r="D57" s="2">
+        <v>43417</v>
+      </c>
+      <c r="E57" s="2">
+        <v>43417</v>
+      </c>
       <c r="F57">
         <v>17</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>22</v>
       </c>
@@ -1962,11 +2056,20 @@
       <c r="C58" t="s">
         <v>4</v>
       </c>
+      <c r="D58" s="2">
+        <v>43417</v>
+      </c>
+      <c r="E58" s="2">
+        <v>43417</v>
+      </c>
       <c r="F58">
         <v>16</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -1976,11 +2079,20 @@
       <c r="C59" t="s">
         <v>4</v>
       </c>
+      <c r="D59" s="2">
+        <v>43417</v>
+      </c>
+      <c r="E59" s="2">
+        <v>43417</v>
+      </c>
       <c r="F59">
         <v>16</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>126</v>
       </c>
@@ -1990,12 +2102,20 @@
       <c r="C60" t="s">
         <v>4</v>
       </c>
-      <c r="D60" s="2"/>
+      <c r="D60" s="2">
+        <v>43417</v>
+      </c>
+      <c r="E60" s="2">
+        <v>43417</v>
+      </c>
       <c r="F60">
         <v>16</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -2005,11 +2125,20 @@
       <c r="C61" t="s">
         <v>4</v>
       </c>
+      <c r="D61" s="2">
+        <v>43417</v>
+      </c>
+      <c r="E61" s="2">
+        <v>43417</v>
+      </c>
       <c r="F61">
         <v>15</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>56</v>
       </c>
@@ -2019,11 +2148,20 @@
       <c r="C62" t="s">
         <v>4</v>
       </c>
+      <c r="D62" s="2">
+        <v>43417</v>
+      </c>
+      <c r="E62" s="2">
+        <v>43417</v>
+      </c>
       <c r="F62">
         <v>14</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>198</v>
       </c>
@@ -2033,13 +2171,20 @@
       <c r="C63" t="s">
         <v>4</v>
       </c>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
+      <c r="D63" s="2">
+        <v>43417</v>
+      </c>
+      <c r="E63" s="2">
+        <v>43417</v>
+      </c>
       <c r="F63">
         <v>11</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>234</v>
       </c>
@@ -2049,10 +2194,17 @@
       <c r="C64" t="s">
         <v>4</v>
       </c>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
+      <c r="D64" s="2">
+        <v>43417</v>
+      </c>
+      <c r="E64" s="2">
+        <v>43417</v>
+      </c>
       <c r="F64">
         <v>11</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
@@ -2065,8 +2217,17 @@
       <c r="C65" t="s">
         <v>4</v>
       </c>
+      <c r="D65" s="2">
+        <v>43417</v>
+      </c>
+      <c r="E65" s="2">
+        <v>43417</v>
+      </c>
       <c r="F65">
         <v>10</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -2079,8 +2240,17 @@
       <c r="C66" t="s">
         <v>4</v>
       </c>
+      <c r="D66" s="2">
+        <v>43417</v>
+      </c>
+      <c r="E66" s="2">
+        <v>43417</v>
+      </c>
       <c r="F66">
         <v>10</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -2093,10 +2263,17 @@
       <c r="C67" t="s">
         <v>4</v>
       </c>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
+      <c r="D67" s="2">
+        <v>43417</v>
+      </c>
+      <c r="E67" s="2">
+        <v>43417</v>
+      </c>
       <c r="F67">
         <v>10</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -2109,8 +2286,17 @@
       <c r="C68" t="s">
         <v>4</v>
       </c>
+      <c r="D68" s="2">
+        <v>43417</v>
+      </c>
+      <c r="E68" s="2">
+        <v>43417</v>
+      </c>
       <c r="F68">
         <v>10</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -2123,8 +2309,17 @@
       <c r="C69" t="s">
         <v>4</v>
       </c>
+      <c r="D69" s="2">
+        <v>43417</v>
+      </c>
+      <c r="E69" s="2">
+        <v>43417</v>
+      </c>
       <c r="F69">
         <v>9</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -2137,8 +2332,17 @@
       <c r="C70" t="s">
         <v>4</v>
       </c>
+      <c r="D70" s="2">
+        <v>43417</v>
+      </c>
+      <c r="E70" s="2">
+        <v>43417</v>
+      </c>
       <c r="F70">
         <v>9</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
@@ -2151,10 +2355,17 @@
       <c r="C71" t="s">
         <v>4</v>
       </c>
-      <c r="D71" s="2"/>
-      <c r="E71" s="2"/>
+      <c r="D71" s="2">
+        <v>43417</v>
+      </c>
+      <c r="E71" s="2">
+        <v>43417</v>
+      </c>
       <c r="F71">
         <v>8</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update lit review progress
</commit_message>
<xml_diff>
--- a/systematic lit review progress notes.xlsx
+++ b/systematic lit review progress notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherineschluth/bansallab/humanhelminths/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D7E2777-B805-B445-88F8-95763E7FFC0C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADFEFCA5-60D8-7548-94BD-E07217EF665A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="460" windowWidth="27640" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="243">
   <si>
     <t>references</t>
   </si>
@@ -741,13 +741,19 @@
     <t>date finished</t>
   </si>
   <si>
-    <t>number of unfiltered results</t>
-  </si>
-  <si>
-    <t>number included in dataset</t>
-  </si>
-  <si>
     <t>comments</t>
+  </si>
+  <si>
+    <t>number of unfiltered results (PMC)</t>
+  </si>
+  <si>
+    <t>number included in dataset (PMC)</t>
+  </si>
+  <si>
+    <t>number of unfiltered results (PubMed)</t>
+  </si>
+  <si>
+    <t>number included in dataset (PubMed)</t>
   </si>
 </sst>
 </file>
@@ -783,10 +789,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1101,10 +1108,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H233"/>
+  <dimension ref="A1:L233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="K188" sqref="K188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1114,7 +1121,7 @@
     <col min="7" max="7" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1131,16 +1138,28 @@
         <v>237</v>
       </c>
       <c r="F1" t="s">
+        <v>239</v>
+      </c>
+      <c r="G1" t="s">
+        <v>240</v>
+      </c>
+      <c r="H1" t="s">
+        <v>236</v>
+      </c>
+      <c r="I1" t="s">
+        <v>237</v>
+      </c>
+      <c r="J1" t="s">
+        <v>241</v>
+      </c>
+      <c r="K1" t="s">
+        <v>242</v>
+      </c>
+      <c r="L1" t="s">
         <v>238</v>
       </c>
-      <c r="G1" t="s">
-        <v>239</v>
-      </c>
-      <c r="H1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1157,10 +1176,10 @@
         <v>2319</v>
       </c>
       <c r="G2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1174,7 +1193,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1191,10 +1210,10 @@
         <v>948</v>
       </c>
       <c r="G4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1211,10 +1230,10 @@
         <v>705</v>
       </c>
       <c r="G5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1224,11 +1243,17 @@
       <c r="C6" t="s">
         <v>4</v>
       </c>
+      <c r="D6" s="2">
+        <v>43427</v>
+      </c>
       <c r="F6">
         <v>667</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1245,10 +1270,10 @@
         <v>654</v>
       </c>
       <c r="G7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1258,11 +1283,17 @@
       <c r="C8" t="s">
         <v>4</v>
       </c>
+      <c r="D8" s="2">
+        <v>43427</v>
+      </c>
       <c r="F8">
         <v>608</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1272,11 +1303,17 @@
       <c r="C9" t="s">
         <v>4</v>
       </c>
+      <c r="D9" s="2">
+        <v>43427</v>
+      </c>
       <c r="F9">
         <v>411</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1293,10 +1330,10 @@
         <v>409</v>
       </c>
       <c r="G10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1310,7 +1347,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1324,7 +1361,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1344,7 +1381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1358,7 +1395,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1372,7 +1409,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1396,8 +1433,14 @@
       <c r="C17" t="s">
         <v>4</v>
       </c>
+      <c r="D17" s="2">
+        <v>43427</v>
+      </c>
       <c r="F17">
         <v>243</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1424,8 +1467,14 @@
       <c r="C19" t="s">
         <v>4</v>
       </c>
+      <c r="D19" s="2">
+        <v>43420</v>
+      </c>
       <c r="F19">
         <v>219</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1452,8 +1501,14 @@
       <c r="C21" t="s">
         <v>4</v>
       </c>
+      <c r="D21" s="2">
+        <v>43427</v>
+      </c>
       <c r="F21">
         <v>186</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1573,8 +1628,15 @@
       <c r="C29" t="s">
         <v>4</v>
       </c>
+      <c r="D29" s="2">
+        <v>43427</v>
+      </c>
+      <c r="E29" s="2"/>
       <c r="F29">
         <v>86</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1620,7 +1682,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -1634,7 +1696,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>27</v>
       </c>
@@ -1648,7 +1710,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -1662,7 +1724,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -1676,7 +1738,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>21</v>
       </c>
@@ -1696,7 +1758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -1706,11 +1768,17 @@
       <c r="C38" t="s">
         <v>4</v>
       </c>
+      <c r="D38" s="2">
+        <v>43427</v>
+      </c>
       <c r="F38">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -1720,11 +1788,17 @@
       <c r="C39" t="s">
         <v>4</v>
       </c>
+      <c r="D39" s="2">
+        <v>43420</v>
+      </c>
       <c r="F39">
         <v>36</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>100</v>
       </c>
@@ -1737,14 +1811,17 @@
       <c r="D40" s="2">
         <v>43417</v>
       </c>
+      <c r="E40" s="2">
+        <v>43431</v>
+      </c>
       <c r="F40">
         <v>35</v>
       </c>
       <c r="G40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>35</v>
       </c>
@@ -1767,7 +1844,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>32</v>
       </c>
@@ -1780,6 +1857,9 @@
       <c r="D42" s="2">
         <v>43417</v>
       </c>
+      <c r="E42" s="2">
+        <v>43431</v>
+      </c>
       <c r="F42">
         <v>34</v>
       </c>
@@ -1787,7 +1867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>60</v>
       </c>
@@ -1800,14 +1880,17 @@
       <c r="D43" s="2">
         <v>43417</v>
       </c>
+      <c r="E43" s="2">
+        <v>43427</v>
+      </c>
       <c r="F43">
         <v>32</v>
       </c>
       <c r="G43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>28</v>
       </c>
@@ -1817,11 +1900,20 @@
       <c r="C44" t="s">
         <v>4</v>
       </c>
+      <c r="D44" s="2">
+        <v>43427</v>
+      </c>
+      <c r="E44" s="2">
+        <v>43427</v>
+      </c>
       <c r="F44">
         <v>25</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>124</v>
       </c>
@@ -1831,12 +1923,20 @@
       <c r="C45" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="2"/>
+      <c r="D45" s="2">
+        <v>43427</v>
+      </c>
+      <c r="E45" s="2">
+        <v>43427</v>
+      </c>
       <c r="F45">
         <v>22</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>57</v>
       </c>
@@ -1846,11 +1946,26 @@
       <c r="C46" t="s">
         <v>4</v>
       </c>
+      <c r="D46" s="2">
+        <v>43424</v>
+      </c>
+      <c r="E46" s="2">
+        <v>43424</v>
+      </c>
       <c r="F46">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46" s="2">
+        <v>43417</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>108</v>
       </c>
@@ -1860,13 +1975,20 @@
       <c r="C47" t="s">
         <v>4</v>
       </c>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
+      <c r="D47" s="2">
+        <v>43424</v>
+      </c>
+      <c r="E47" s="2">
+        <v>43424</v>
+      </c>
       <c r="F47">
         <v>21</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>148</v>
       </c>
@@ -1876,9 +1998,17 @@
       <c r="C48" t="s">
         <v>4</v>
       </c>
-      <c r="D48" s="2"/>
+      <c r="D48" s="2">
+        <v>43424</v>
+      </c>
+      <c r="E48" s="2">
+        <v>43424</v>
+      </c>
       <c r="F48">
         <v>21</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -1891,8 +2021,17 @@
       <c r="C49" t="s">
         <v>4</v>
       </c>
+      <c r="D49" s="2">
+        <v>43424</v>
+      </c>
+      <c r="E49" s="2">
+        <v>43424</v>
+      </c>
       <c r="F49">
         <v>20</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -1905,9 +2044,17 @@
       <c r="C50" t="s">
         <v>4</v>
       </c>
-      <c r="D50" s="2"/>
+      <c r="D50" s="2">
+        <v>43420</v>
+      </c>
+      <c r="E50" s="2">
+        <v>43420</v>
+      </c>
       <c r="F50">
         <v>19</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -1920,9 +2067,17 @@
       <c r="C51" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="2"/>
+      <c r="D51" s="2">
+        <v>43420</v>
+      </c>
+      <c r="E51" s="2">
+        <v>43420</v>
+      </c>
       <c r="F51">
         <v>19</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
@@ -1935,8 +2090,17 @@
       <c r="C52" t="s">
         <v>4</v>
       </c>
+      <c r="D52" s="2">
+        <v>43420</v>
+      </c>
+      <c r="E52" s="2">
+        <v>43420</v>
+      </c>
       <c r="F52">
         <v>19</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -1949,9 +2113,17 @@
       <c r="C53" t="s">
         <v>4</v>
       </c>
-      <c r="D53" s="2"/>
+      <c r="D53" s="2">
+        <v>43420</v>
+      </c>
+      <c r="E53" s="2">
+        <v>43420</v>
+      </c>
       <c r="F53">
         <v>18</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -4783,7 +4955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>177</v>
       </c>
@@ -4806,7 +4978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>153</v>
       </c>
@@ -4829,7 +5001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>129</v>
       </c>
@@ -4852,7 +5024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>178</v>
       </c>
@@ -4875,7 +5047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>46</v>
       </c>
@@ -4898,7 +5070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>87</v>
       </c>
@@ -4921,7 +5093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>48</v>
       </c>
@@ -4944,7 +5116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>88</v>
       </c>
@@ -4967,7 +5139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>119</v>
       </c>
@@ -4990,7 +5162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>154</v>
       </c>
@@ -5013,7 +5185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>130</v>
       </c>
@@ -5036,7 +5208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>180</v>
       </c>
@@ -5059,7 +5231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>224</v>
       </c>
@@ -5081,8 +5253,14 @@
       <c r="G189">
         <v>0</v>
       </c>
-    </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J189">
+        <v>0</v>
+      </c>
+      <c r="K189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>106</v>
       </c>
@@ -5104,8 +5282,14 @@
       <c r="G190">
         <v>0</v>
       </c>
-    </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J190">
+        <v>0</v>
+      </c>
+      <c r="K190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>72</v>
       </c>
@@ -5127,8 +5311,14 @@
       <c r="G191">
         <v>0</v>
       </c>
-    </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J191">
+        <v>0</v>
+      </c>
+      <c r="K191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>182</v>
       </c>
@@ -5150,8 +5340,14 @@
       <c r="G192">
         <v>0</v>
       </c>
-    </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J192">
+        <v>0</v>
+      </c>
+      <c r="K192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>225</v>
       </c>
@@ -5173,8 +5369,14 @@
       <c r="G193">
         <v>0</v>
       </c>
-    </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J193">
+        <v>0</v>
+      </c>
+      <c r="K193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>54</v>
       </c>
@@ -5196,8 +5398,14 @@
       <c r="G194">
         <v>0</v>
       </c>
-    </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J194">
+        <v>0</v>
+      </c>
+      <c r="K194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>73</v>
       </c>
@@ -5219,8 +5427,14 @@
       <c r="G195">
         <v>0</v>
       </c>
-    </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J195">
+        <v>0</v>
+      </c>
+      <c r="K195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>131</v>
       </c>
@@ -5242,8 +5456,14 @@
       <c r="G196">
         <v>0</v>
       </c>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J196">
+        <v>0</v>
+      </c>
+      <c r="K196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>67</v>
       </c>
@@ -5265,8 +5485,14 @@
       <c r="G197">
         <v>0</v>
       </c>
-    </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J197">
+        <v>0</v>
+      </c>
+      <c r="K197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>209</v>
       </c>
@@ -5288,8 +5514,14 @@
       <c r="G198">
         <v>0</v>
       </c>
-    </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J198">
+        <v>0</v>
+      </c>
+      <c r="K198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>183</v>
       </c>
@@ -5311,8 +5543,14 @@
       <c r="G199">
         <v>0</v>
       </c>
-    </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J199">
+        <v>0</v>
+      </c>
+      <c r="K199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>107</v>
       </c>
@@ -5334,8 +5572,14 @@
       <c r="G200">
         <v>0</v>
       </c>
-    </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J200">
+        <v>0</v>
+      </c>
+      <c r="K200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>139</v>
       </c>
@@ -5357,8 +5601,14 @@
       <c r="G201" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J201">
+        <v>0</v>
+      </c>
+      <c r="K201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>156</v>
       </c>
@@ -5380,8 +5630,14 @@
       <c r="G202">
         <v>0</v>
       </c>
-    </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J202">
+        <v>0</v>
+      </c>
+      <c r="K202">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>184</v>
       </c>
@@ -5403,8 +5659,14 @@
       <c r="G203">
         <v>0</v>
       </c>
-    </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J203">
+        <v>0</v>
+      </c>
+      <c r="K203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>159</v>
       </c>
@@ -5426,8 +5688,14 @@
       <c r="G204">
         <v>0</v>
       </c>
-    </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J204">
+        <v>0</v>
+      </c>
+      <c r="K204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>210</v>
       </c>
@@ -5449,8 +5717,14 @@
       <c r="G205">
         <v>0</v>
       </c>
-    </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J205">
+        <v>0</v>
+      </c>
+      <c r="K205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>141</v>
       </c>
@@ -5472,8 +5746,14 @@
       <c r="G206">
         <v>0</v>
       </c>
-    </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J206">
+        <v>0</v>
+      </c>
+      <c r="K206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>187</v>
       </c>
@@ -5495,8 +5775,14 @@
       <c r="G207">
         <v>0</v>
       </c>
-    </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J207">
+        <v>0</v>
+      </c>
+      <c r="K207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>211</v>
       </c>
@@ -5518,8 +5804,14 @@
       <c r="G208">
         <v>0</v>
       </c>
-    </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J208">
+        <v>0</v>
+      </c>
+      <c r="K208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>160</v>
       </c>
@@ -5541,8 +5833,14 @@
       <c r="G209">
         <v>0</v>
       </c>
-    </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J209">
+        <v>0</v>
+      </c>
+      <c r="K209">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>188</v>
       </c>
@@ -5564,8 +5862,14 @@
       <c r="G210">
         <v>0</v>
       </c>
-    </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J210">
+        <v>0</v>
+      </c>
+      <c r="K210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>212</v>
       </c>
@@ -5587,8 +5891,14 @@
       <c r="G211">
         <v>0</v>
       </c>
-    </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J211">
+        <v>0</v>
+      </c>
+      <c r="K211">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>229</v>
       </c>
@@ -5610,8 +5920,14 @@
       <c r="G212">
         <v>0</v>
       </c>
-    </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J212">
+        <v>0</v>
+      </c>
+      <c r="K212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>192</v>
       </c>
@@ -5633,8 +5949,14 @@
       <c r="G213">
         <v>0</v>
       </c>
-    </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J213">
+        <v>0</v>
+      </c>
+      <c r="K213">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>162</v>
       </c>
@@ -5656,8 +5978,14 @@
       <c r="G214">
         <v>0</v>
       </c>
-    </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J214">
+        <v>0</v>
+      </c>
+      <c r="K214">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>230</v>
       </c>
@@ -5679,8 +6007,14 @@
       <c r="G215">
         <v>0</v>
       </c>
-    </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J215">
+        <v>0</v>
+      </c>
+      <c r="K215">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>142</v>
       </c>
@@ -5702,8 +6036,14 @@
       <c r="G216">
         <v>0</v>
       </c>
-    </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J216">
+        <v>0</v>
+      </c>
+      <c r="K216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>110</v>
       </c>
@@ -5725,8 +6065,14 @@
       <c r="G217">
         <v>0</v>
       </c>
-    </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J217">
+        <v>0</v>
+      </c>
+      <c r="K217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>163</v>
       </c>
@@ -5748,8 +6094,14 @@
       <c r="G218">
         <v>0</v>
       </c>
-    </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J218">
+        <v>0</v>
+      </c>
+      <c r="K218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>143</v>
       </c>
@@ -5771,8 +6123,14 @@
       <c r="G219">
         <v>0</v>
       </c>
-    </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J219">
+        <v>0</v>
+      </c>
+      <c r="K219">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>193</v>
       </c>
@@ -5794,8 +6152,14 @@
       <c r="G220">
         <v>0</v>
       </c>
-    </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J220">
+        <v>0</v>
+      </c>
+      <c r="K220">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>144</v>
       </c>
@@ -5817,8 +6181,14 @@
       <c r="G221">
         <v>0</v>
       </c>
-    </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J221">
+        <v>0</v>
+      </c>
+      <c r="K221">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>215</v>
       </c>
@@ -5840,8 +6210,14 @@
       <c r="G222">
         <v>0</v>
       </c>
-    </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J222">
+        <v>0</v>
+      </c>
+      <c r="K222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>122</v>
       </c>
@@ -5863,8 +6239,14 @@
       <c r="G223">
         <v>0</v>
       </c>
-    </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J223">
+        <v>0</v>
+      </c>
+      <c r="K223">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>194</v>
       </c>
@@ -5886,8 +6268,14 @@
       <c r="G224">
         <v>0</v>
       </c>
-    </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J224">
+        <v>0</v>
+      </c>
+      <c r="K224">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>195</v>
       </c>
@@ -5909,8 +6297,14 @@
       <c r="G225">
         <v>0</v>
       </c>
-    </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J225">
+        <v>0</v>
+      </c>
+      <c r="K225">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>231</v>
       </c>
@@ -5932,8 +6326,14 @@
       <c r="G226">
         <v>0</v>
       </c>
-    </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J226">
+        <v>0</v>
+      </c>
+      <c r="K226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>92</v>
       </c>
@@ -5955,8 +6355,14 @@
       <c r="G227">
         <v>0</v>
       </c>
-    </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J227">
+        <v>0</v>
+      </c>
+      <c r="K227">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>197</v>
       </c>
@@ -5978,8 +6384,14 @@
       <c r="G228">
         <v>0</v>
       </c>
-    </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J228">
+        <v>0</v>
+      </c>
+      <c r="K228">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>147</v>
       </c>
@@ -6001,8 +6413,14 @@
       <c r="G229">
         <v>0</v>
       </c>
-    </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J229">
+        <v>0</v>
+      </c>
+      <c r="K229">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>199</v>
       </c>
@@ -6024,8 +6442,14 @@
       <c r="G230">
         <v>0</v>
       </c>
-    </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J230">
+        <v>0</v>
+      </c>
+      <c r="K230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>217</v>
       </c>
@@ -6047,8 +6471,20 @@
       <c r="G231">
         <v>0</v>
       </c>
-    </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H231" s="2">
+        <v>43431</v>
+      </c>
+      <c r="I231" s="2">
+        <v>43431</v>
+      </c>
+      <c r="J231">
+        <v>0</v>
+      </c>
+      <c r="K231">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>113</v>
       </c>
@@ -6070,8 +6506,20 @@
       <c r="G232">
         <v>0</v>
       </c>
-    </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H232" s="2">
+        <v>43431</v>
+      </c>
+      <c r="I232" s="2">
+        <v>43431</v>
+      </c>
+      <c r="J232" s="3">
+        <v>0</v>
+      </c>
+      <c r="K232" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>201</v>
       </c>
@@ -6091,6 +6539,18 @@
         <v>0</v>
       </c>
       <c r="G233">
+        <v>0</v>
+      </c>
+      <c r="H233" s="2">
+        <v>43431</v>
+      </c>
+      <c r="I233" s="2">
+        <v>43431</v>
+      </c>
+      <c r="J233" s="3">
+        <v>0</v>
+      </c>
+      <c r="K233" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated lit review progress
</commit_message>
<xml_diff>
--- a/systematic lit review progress notes.xlsx
+++ b/systematic lit review progress notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherineschluth/bansallab/humanhelminths/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD64D314-ED53-F14D-B8C2-D88169DD8FA6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE53EB66-5179-6D43-B142-D1FE1DAFA350}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="460" windowWidth="27640" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -769,12 +769,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -789,11 +801,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1110,8 +1124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="M151" sqref="M151"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K141" sqref="K141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1176,7 +1190,10 @@
         <v>2319</v>
       </c>
       <c r="G2">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="J2">
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -1192,6 +1209,9 @@
       <c r="F3">
         <v>977</v>
       </c>
+      <c r="J3">
+        <v>58</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1212,6 +1232,9 @@
       <c r="G4">
         <v>2</v>
       </c>
+      <c r="J4">
+        <v>80</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1230,7 +1253,10 @@
         <v>705</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="J5">
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1252,6 +1278,9 @@
       <c r="G6">
         <v>1</v>
       </c>
+      <c r="J6">
+        <v>74</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1272,6 +1301,9 @@
       <c r="G7">
         <v>2</v>
       </c>
+      <c r="J7">
+        <v>58</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1292,6 +1324,9 @@
       <c r="G8">
         <v>2</v>
       </c>
+      <c r="J8">
+        <v>42</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1310,7 +1345,10 @@
         <v>411</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -1332,6 +1370,9 @@
       <c r="G10">
         <v>2</v>
       </c>
+      <c r="J10">
+        <v>36</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1346,6 +1387,9 @@
       <c r="F11">
         <v>404</v>
       </c>
+      <c r="J11">
+        <v>28</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1360,6 +1404,9 @@
       <c r="F12">
         <v>382</v>
       </c>
+      <c r="J12">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1378,7 +1425,10 @@
         <v>320</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -1391,8 +1441,17 @@
       <c r="C14" t="s">
         <v>4</v>
       </c>
+      <c r="D14" s="2">
+        <v>43438</v>
+      </c>
       <c r="F14">
         <v>283</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -1408,6 +1467,9 @@
       <c r="F15">
         <v>270</v>
       </c>
+      <c r="J15">
+        <v>31</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1419,11 +1481,20 @@
       <c r="C16" t="s">
         <v>4</v>
       </c>
+      <c r="D16" s="2">
+        <v>43432</v>
+      </c>
       <c r="F16">
         <v>265</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="J16">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1440,10 +1511,13 @@
         <v>243</v>
       </c>
       <c r="G17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1456,8 +1530,11 @@
       <c r="F18">
         <v>219</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1476,8 +1553,11 @@
       <c r="G19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -1490,8 +1570,11 @@
       <c r="F20">
         <v>190</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1510,8 +1593,11 @@
       <c r="G21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J21">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1524,8 +1610,20 @@
       <c r="F22">
         <v>167</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H22" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I22" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -1538,8 +1636,11 @@
       <c r="F23">
         <v>131</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>102</v>
       </c>
@@ -1553,8 +1654,11 @@
       <c r="F24">
         <v>112</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>114</v>
       </c>
@@ -1568,8 +1672,20 @@
       <c r="F25">
         <v>112</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H25" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I25" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -1588,8 +1704,11 @@
       <c r="G26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>101</v>
       </c>
@@ -1603,8 +1722,11 @@
       <c r="F27">
         <v>90</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -1617,8 +1739,11 @@
       <c r="F28">
         <v>87</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -1638,8 +1763,11 @@
       <c r="G29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1652,8 +1780,11 @@
       <c r="F30">
         <v>67</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>168</v>
       </c>
@@ -1667,8 +1798,11 @@
       <c r="F31">
         <v>61</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>25</v>
       </c>
@@ -1680,6 +1814,9 @@
       </c>
       <c r="F32">
         <v>59</v>
+      </c>
+      <c r="J32">
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -1692,8 +1829,29 @@
       <c r="C33" t="s">
         <v>4</v>
       </c>
+      <c r="D33" s="2">
+        <v>43438</v>
+      </c>
+      <c r="E33" s="2">
+        <v>43438</v>
+      </c>
       <c r="F33">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I33" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -1706,8 +1864,20 @@
       <c r="C34" t="s">
         <v>4</v>
       </c>
+      <c r="D34" s="2">
+        <v>43437</v>
+      </c>
+      <c r="E34" s="2">
+        <v>43437</v>
+      </c>
       <c r="F34">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
@@ -1720,8 +1890,20 @@
       <c r="C35" t="s">
         <v>4</v>
       </c>
+      <c r="D35" s="2">
+        <v>43437</v>
+      </c>
+      <c r="E35" s="2">
+        <v>43437</v>
+      </c>
       <c r="F35">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -1734,8 +1916,20 @@
       <c r="C36" t="s">
         <v>4</v>
       </c>
+      <c r="D36" s="2">
+        <v>43436</v>
+      </c>
+      <c r="E36" s="2">
+        <v>43436</v>
+      </c>
       <c r="F36">
         <v>38</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -1751,11 +1945,17 @@
       <c r="D37" s="2">
         <v>43417</v>
       </c>
+      <c r="E37" s="2">
+        <v>43436</v>
+      </c>
       <c r="F37">
         <v>37</v>
       </c>
       <c r="G37">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="J37">
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -1771,11 +1971,17 @@
       <c r="D38" s="2">
         <v>43427</v>
       </c>
+      <c r="E38" s="2">
+        <v>43436</v>
+      </c>
       <c r="F38">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G38">
         <v>1</v>
+      </c>
+      <c r="J38">
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -1791,11 +1997,17 @@
       <c r="D39" s="2">
         <v>43420</v>
       </c>
+      <c r="E39" s="2">
+        <v>43436</v>
+      </c>
       <c r="F39">
         <v>36</v>
       </c>
       <c r="G39">
         <v>1</v>
+      </c>
+      <c r="J39">
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -1820,6 +2032,18 @@
       <c r="G40">
         <v>2</v>
       </c>
+      <c r="H40" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I40" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
@@ -1843,6 +2067,18 @@
       <c r="G41">
         <v>3</v>
       </c>
+      <c r="H41" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I41" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
@@ -1866,6 +2102,18 @@
       <c r="G42">
         <v>2</v>
       </c>
+      <c r="H42" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I42" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
@@ -1889,6 +2137,18 @@
       <c r="G43">
         <v>2</v>
       </c>
+      <c r="H43" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I43" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
@@ -1912,6 +2172,18 @@
       <c r="G44">
         <v>1</v>
       </c>
+      <c r="H44" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I44" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
@@ -1935,6 +2207,18 @@
       <c r="G45">
         <v>0</v>
       </c>
+      <c r="H45" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I45" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
@@ -1961,7 +2245,13 @@
       <c r="H46" s="2">
         <v>43417</v>
       </c>
-      <c r="K46">
+      <c r="I46" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46" s="5">
         <v>1</v>
       </c>
     </row>
@@ -1987,6 +2277,18 @@
       <c r="G47">
         <v>0</v>
       </c>
+      <c r="H47" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I47" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
@@ -2010,8 +2312,20 @@
       <c r="G48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H48" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I48" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>69</v>
       </c>
@@ -2033,8 +2347,20 @@
       <c r="G49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H49" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I49" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J49">
+        <v>3</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>111</v>
       </c>
@@ -2056,8 +2382,20 @@
       <c r="G50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H50" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I50" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>125</v>
       </c>
@@ -2079,8 +2417,20 @@
       <c r="G51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H51" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I51" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J51">
+        <v>3</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -2102,8 +2452,20 @@
       <c r="G52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H52" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I52" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J52">
+        <v>1</v>
+      </c>
+      <c r="K52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>167</v>
       </c>
@@ -2125,8 +2487,20 @@
       <c r="G53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H53" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I53" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>103</v>
       </c>
@@ -2148,8 +2522,20 @@
       <c r="G54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H54" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I54" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>158</v>
       </c>
@@ -2171,8 +2557,20 @@
       <c r="G55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H55" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I55" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>196</v>
       </c>
@@ -2194,8 +2592,20 @@
       <c r="G56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H56" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I56" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>202</v>
       </c>
@@ -2217,8 +2627,20 @@
       <c r="G57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H57" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I57" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>22</v>
       </c>
@@ -2240,8 +2662,11 @@
       <c r="G58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -2263,8 +2688,11 @@
       <c r="G59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>126</v>
       </c>
@@ -2286,8 +2714,11 @@
       <c r="G60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -2309,8 +2740,12 @@
       <c r="G61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I61" s="2"/>
+      <c r="J61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>56</v>
       </c>
@@ -2332,8 +2767,20 @@
       <c r="G62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H62" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I62" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="K62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>198</v>
       </c>
@@ -2355,8 +2802,20 @@
       <c r="G63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H63" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I63" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>234</v>
       </c>
@@ -2378,8 +2837,20 @@
       <c r="G64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H64" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I64" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="K64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>47</v>
       </c>
@@ -2401,8 +2872,20 @@
       <c r="G65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H65" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I65" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>97</v>
       </c>
@@ -2424,8 +2907,20 @@
       <c r="G66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H66" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I66" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>189</v>
       </c>
@@ -2447,8 +2942,20 @@
       <c r="G67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H67" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I67" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>45</v>
       </c>
@@ -2470,8 +2977,20 @@
       <c r="G68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H68" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I68" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J68">
+        <v>0</v>
+      </c>
+      <c r="K68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>41</v>
       </c>
@@ -2493,8 +3012,20 @@
       <c r="G69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H69" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I69" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+      <c r="K69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>65</v>
       </c>
@@ -2516,8 +3047,11 @@
       <c r="G70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J70">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>219</v>
       </c>
@@ -2539,8 +3073,20 @@
       <c r="G71">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H71" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I71" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J71">
+        <v>2</v>
+      </c>
+      <c r="K71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>228</v>
       </c>
@@ -2562,8 +3108,20 @@
       <c r="G72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H72" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I72" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+      <c r="K72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>172</v>
       </c>
@@ -2585,8 +3143,20 @@
       <c r="G73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H73" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I73" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+      <c r="K73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>42</v>
       </c>
@@ -2608,8 +3178,20 @@
       <c r="G74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H74" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I74" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J74">
+        <v>1</v>
+      </c>
+      <c r="K74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>84</v>
       </c>
@@ -2631,8 +3213,20 @@
       <c r="G75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H75" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I75" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+      <c r="K75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>37</v>
       </c>
@@ -2654,8 +3248,20 @@
       <c r="G76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H76" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I76" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J76">
+        <v>0</v>
+      </c>
+      <c r="K76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>30</v>
       </c>
@@ -2677,8 +3283,20 @@
       <c r="G77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H77" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I77" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J77">
+        <v>0</v>
+      </c>
+      <c r="K77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>98</v>
       </c>
@@ -2700,8 +3318,20 @@
       <c r="G78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H78" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I78" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J78">
+        <v>0</v>
+      </c>
+      <c r="K78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>109</v>
       </c>
@@ -2723,8 +3353,20 @@
       <c r="G79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H79" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I79" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J79">
+        <v>1</v>
+      </c>
+      <c r="K79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>190</v>
       </c>
@@ -2746,8 +3388,20 @@
       <c r="G80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H80" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I80" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J80">
+        <v>0</v>
+      </c>
+      <c r="K80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>165</v>
       </c>
@@ -2769,8 +3423,20 @@
       <c r="G81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H81" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I81" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J81">
+        <v>0</v>
+      </c>
+      <c r="K81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>112</v>
       </c>
@@ -2792,8 +3458,20 @@
       <c r="G82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H82" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I82" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J82">
+        <v>0</v>
+      </c>
+      <c r="K82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>58</v>
       </c>
@@ -2815,8 +3493,20 @@
       <c r="G83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H83" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I83" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J83">
+        <v>1</v>
+      </c>
+      <c r="K83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>140</v>
       </c>
@@ -2838,8 +3528,20 @@
       <c r="G84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H84" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I84" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J84">
+        <v>1</v>
+      </c>
+      <c r="K84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>191</v>
       </c>
@@ -2861,8 +3563,20 @@
       <c r="G85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H85" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I85" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J85">
+        <v>0</v>
+      </c>
+      <c r="K85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>146</v>
       </c>
@@ -2884,8 +3598,20 @@
       <c r="G86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H86" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I86" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J86">
+        <v>0</v>
+      </c>
+      <c r="K86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>232</v>
       </c>
@@ -2907,8 +3633,20 @@
       <c r="G87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H87" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I87" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J87">
+        <v>0</v>
+      </c>
+      <c r="K87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>44</v>
       </c>
@@ -2930,8 +3668,20 @@
       <c r="G88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H88" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I88" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J88">
+        <v>0</v>
+      </c>
+      <c r="K88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>116</v>
       </c>
@@ -2953,8 +3703,20 @@
       <c r="G89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H89" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I89" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J89">
+        <v>0</v>
+      </c>
+      <c r="K89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>223</v>
       </c>
@@ -2976,8 +3738,20 @@
       <c r="G90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H90" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I90" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J90">
+        <v>0</v>
+      </c>
+      <c r="K90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>96</v>
       </c>
@@ -2999,8 +3773,20 @@
       <c r="G91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H91" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I91" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J91">
+        <v>0</v>
+      </c>
+      <c r="K91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>208</v>
       </c>
@@ -3022,8 +3808,20 @@
       <c r="G92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H92" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I92" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J92">
+        <v>0</v>
+      </c>
+      <c r="K92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>133</v>
       </c>
@@ -3045,8 +3843,20 @@
       <c r="G93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H93" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I93" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J93">
+        <v>0</v>
+      </c>
+      <c r="K93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>99</v>
       </c>
@@ -3068,8 +3878,20 @@
       <c r="G94">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H94" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I94" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J94">
+        <v>0</v>
+      </c>
+      <c r="K94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>90</v>
       </c>
@@ -3091,8 +3913,20 @@
       <c r="G95">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H95" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I95" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J95">
+        <v>0</v>
+      </c>
+      <c r="K95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>166</v>
       </c>
@@ -3114,8 +3948,20 @@
       <c r="G96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H96" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I96" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J96">
+        <v>0</v>
+      </c>
+      <c r="K96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>39</v>
       </c>
@@ -3137,8 +3983,20 @@
       <c r="G97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H97" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I97" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J97">
+        <v>1</v>
+      </c>
+      <c r="K97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>75</v>
       </c>
@@ -3160,8 +4018,20 @@
       <c r="G98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H98" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I98" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J98">
+        <v>0</v>
+      </c>
+      <c r="K98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>115</v>
       </c>
@@ -3183,8 +4053,20 @@
       <c r="G99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H99" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I99" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J99">
+        <v>0</v>
+      </c>
+      <c r="K99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>94</v>
       </c>
@@ -3206,8 +4088,20 @@
       <c r="G100">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H100" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I100" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J100">
+        <v>0</v>
+      </c>
+      <c r="K100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>40</v>
       </c>
@@ -3229,8 +4123,20 @@
       <c r="G101">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H101" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I101" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J101">
+        <v>2</v>
+      </c>
+      <c r="K101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>226</v>
       </c>
@@ -3252,8 +4158,20 @@
       <c r="G102">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H102" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I102" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J102">
+        <v>3</v>
+      </c>
+      <c r="K102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>134</v>
       </c>
@@ -3275,8 +4193,20 @@
       <c r="G103">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H103" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I103" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J103">
+        <v>0</v>
+      </c>
+      <c r="K103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>121</v>
       </c>
@@ -3298,8 +4228,20 @@
       <c r="G104">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H104" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I104" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J104">
+        <v>0</v>
+      </c>
+      <c r="K104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>135</v>
       </c>
@@ -3321,8 +4263,20 @@
       <c r="G105">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H105" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I105" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J105">
+        <v>0</v>
+      </c>
+      <c r="K105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>216</v>
       </c>
@@ -3344,8 +4298,20 @@
       <c r="G106">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H106" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I106" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J106">
+        <v>0</v>
+      </c>
+      <c r="K106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>233</v>
       </c>
@@ -3367,8 +4333,20 @@
       <c r="G107">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H107" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I107" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J107">
+        <v>0</v>
+      </c>
+      <c r="K107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>200</v>
       </c>
@@ -3390,8 +4368,20 @@
       <c r="G108">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H108" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I108" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J108">
+        <v>0</v>
+      </c>
+      <c r="K108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>150</v>
       </c>
@@ -3413,8 +4403,20 @@
       <c r="G109">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H109" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I109" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J109">
+        <v>2</v>
+      </c>
+      <c r="K109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>151</v>
       </c>
@@ -3436,8 +4438,20 @@
       <c r="G110">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H110" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I110" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J110">
+        <v>0</v>
+      </c>
+      <c r="K110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>76</v>
       </c>
@@ -3459,8 +4473,20 @@
       <c r="G111">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H111" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I111" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J111">
+        <v>0</v>
+      </c>
+      <c r="K111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>118</v>
       </c>
@@ -3482,8 +4508,20 @@
       <c r="G112">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H112" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I112" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J112">
+        <v>0</v>
+      </c>
+      <c r="K112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>80</v>
       </c>
@@ -3505,8 +4543,20 @@
       <c r="G113">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H113" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I113" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J113">
+        <v>0</v>
+      </c>
+      <c r="K113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>63</v>
       </c>
@@ -3528,8 +4578,20 @@
       <c r="G114">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H114" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I114" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J114">
+        <v>0</v>
+      </c>
+      <c r="K114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>179</v>
       </c>
@@ -3551,8 +4613,20 @@
       <c r="G115">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H115" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I115" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J115">
+        <v>0</v>
+      </c>
+      <c r="K115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>43</v>
       </c>
@@ -3574,8 +4648,20 @@
       <c r="G116">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H116" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I116" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J116">
+        <v>0</v>
+      </c>
+      <c r="K116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>64</v>
       </c>
@@ -3597,8 +4683,20 @@
       <c r="G117">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H117" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I117" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J117">
+        <v>0</v>
+      </c>
+      <c r="K117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>120</v>
       </c>
@@ -3620,8 +4718,20 @@
       <c r="G118">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H118" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I118" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J118">
+        <v>0</v>
+      </c>
+      <c r="K118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>82</v>
       </c>
@@ -3643,8 +4753,20 @@
       <c r="G119">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H119" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I119" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J119">
+        <v>0</v>
+      </c>
+      <c r="K119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>155</v>
       </c>
@@ -3666,8 +4788,20 @@
       <c r="G120">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H120" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I120" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J120">
+        <v>0</v>
+      </c>
+      <c r="K120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>185</v>
       </c>
@@ -3689,8 +4823,20 @@
       <c r="G121">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H121" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I121" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J121">
+        <v>0</v>
+      </c>
+      <c r="K121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>227</v>
       </c>
@@ -3712,8 +4858,20 @@
       <c r="G122">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H122" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I122" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J122">
+        <v>0</v>
+      </c>
+      <c r="K122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>86</v>
       </c>
@@ -3735,8 +4893,20 @@
       <c r="G123">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H123" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I123" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J123">
+        <v>1</v>
+      </c>
+      <c r="K123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>205</v>
       </c>
@@ -3758,8 +4928,20 @@
       <c r="G124" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H124" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I124" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J124">
+        <v>0</v>
+      </c>
+      <c r="K124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>235</v>
       </c>
@@ -3781,8 +4963,20 @@
       <c r="G125">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H125" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I125" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J125">
+        <v>0</v>
+      </c>
+      <c r="K125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>220</v>
       </c>
@@ -3804,8 +4998,20 @@
       <c r="G126">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H126" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I126" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J126">
+        <v>0</v>
+      </c>
+      <c r="K126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>174</v>
       </c>
@@ -3827,8 +5033,20 @@
       <c r="G127">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H127" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I127" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J127">
+        <v>0</v>
+      </c>
+      <c r="K127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>222</v>
       </c>
@@ -3850,8 +5068,20 @@
       <c r="G128">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H128" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I128" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J128">
+        <v>0</v>
+      </c>
+      <c r="K128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>77</v>
       </c>
@@ -3873,8 +5103,20 @@
       <c r="G129">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H129" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I129" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J129">
+        <v>0</v>
+      </c>
+      <c r="K129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>95</v>
       </c>
@@ -3896,8 +5138,20 @@
       <c r="G130">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H130" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I130" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J130">
+        <v>0</v>
+      </c>
+      <c r="K130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>62</v>
       </c>
@@ -3919,8 +5173,20 @@
       <c r="G131">
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H131" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I131" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J131">
+        <v>0</v>
+      </c>
+      <c r="K131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>52</v>
       </c>
@@ -3942,8 +5208,20 @@
       <c r="G132">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H132" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I132" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J132">
+        <v>0</v>
+      </c>
+      <c r="K132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>181</v>
       </c>
@@ -3965,8 +5243,20 @@
       <c r="G133">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H133" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I133" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J133">
+        <v>0</v>
+      </c>
+      <c r="K133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>89</v>
       </c>
@@ -3988,8 +5278,20 @@
       <c r="G134">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H134" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I134" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J134">
+        <v>0</v>
+      </c>
+      <c r="K134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>66</v>
       </c>
@@ -4011,8 +5313,20 @@
       <c r="G135">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H135" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I135" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J135">
+        <v>0</v>
+      </c>
+      <c r="K135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>81</v>
       </c>
@@ -4034,8 +5348,20 @@
       <c r="G136">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H136" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I136" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J136">
+        <v>0</v>
+      </c>
+      <c r="K136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>157</v>
       </c>
@@ -4057,8 +5383,20 @@
       <c r="G137">
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H137" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I137" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J137">
+        <v>0</v>
+      </c>
+      <c r="K137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>132</v>
       </c>
@@ -4080,8 +5418,20 @@
       <c r="G138">
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H138" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I138" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J138">
+        <v>0</v>
+      </c>
+      <c r="K138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>186</v>
       </c>
@@ -4103,8 +5453,20 @@
       <c r="G139">
         <v>0</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H139" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I139" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J139">
+        <v>0</v>
+      </c>
+      <c r="K139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>161</v>
       </c>
@@ -4126,8 +5488,20 @@
       <c r="G140">
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H140" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I140" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J140">
+        <v>0</v>
+      </c>
+      <c r="K140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>83</v>
       </c>
@@ -4149,8 +5523,20 @@
       <c r="G141">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H141" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I141" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J141">
+        <v>0</v>
+      </c>
+      <c r="K141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>213</v>
       </c>
@@ -4172,8 +5558,20 @@
       <c r="G142">
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H142" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I142" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J142">
+        <v>0</v>
+      </c>
+      <c r="K142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>214</v>
       </c>
@@ -4195,8 +5593,20 @@
       <c r="G143">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H143" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I143" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J143">
+        <v>0</v>
+      </c>
+      <c r="K143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>85</v>
       </c>
@@ -4216,6 +5626,18 @@
         <v>1</v>
       </c>
       <c r="G144">
+        <v>0</v>
+      </c>
+      <c r="H144" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I144" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J144">
+        <v>0</v>
+      </c>
+      <c r="K144">
         <v>0</v>
       </c>
     </row>
@@ -4241,6 +5663,18 @@
       <c r="G145">
         <v>0</v>
       </c>
+      <c r="H145" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I145" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J145">
+        <v>0</v>
+      </c>
+      <c r="K145">
+        <v>0</v>
+      </c>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
@@ -4264,6 +5698,18 @@
       <c r="G146">
         <v>0</v>
       </c>
+      <c r="H146" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I146" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J146">
+        <v>0</v>
+      </c>
+      <c r="K146">
+        <v>0</v>
+      </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
@@ -4287,6 +5733,18 @@
       <c r="G147">
         <v>0</v>
       </c>
+      <c r="H147" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I147" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J147">
+        <v>0</v>
+      </c>
+      <c r="K147">
+        <v>0</v>
+      </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
@@ -4310,6 +5768,18 @@
       <c r="G148">
         <v>0</v>
       </c>
+      <c r="H148" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I148" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J148">
+        <v>0</v>
+      </c>
+      <c r="K148">
+        <v>0</v>
+      </c>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
@@ -4333,6 +5803,18 @@
       <c r="G149">
         <v>0</v>
       </c>
+      <c r="H149" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I149" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J149">
+        <v>0</v>
+      </c>
+      <c r="K149">
+        <v>0</v>
+      </c>
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
@@ -4354,6 +5836,18 @@
         <v>1</v>
       </c>
       <c r="G150">
+        <v>0</v>
+      </c>
+      <c r="H150" s="2">
+        <v>43438</v>
+      </c>
+      <c r="I150" s="2">
+        <v>43438</v>
+      </c>
+      <c r="J150">
+        <v>0</v>
+      </c>
+      <c r="K150">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Slowly but surely plugging along here
</commit_message>
<xml_diff>
--- a/systematic lit review progress notes.xlsx
+++ b/systematic lit review progress notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherineschluth/bansallab/humanhelminths/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE53EB66-5179-6D43-B142-D1FE1DAFA350}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D76E2E87-6306-924A-ACFA-02697D241D00}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1125,7 +1126,7 @@
   <dimension ref="A1:L233"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K141" sqref="K141"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1190,7 +1191,7 @@
         <v>2319</v>
       </c>
       <c r="G2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="J2">
         <v>237</v>
@@ -1206,8 +1207,14 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
+      <c r="D3" s="2">
+        <v>43470</v>
+      </c>
       <c r="F3">
         <v>977</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
       </c>
       <c r="J3">
         <v>58</v>
@@ -1253,7 +1260,7 @@
         <v>705</v>
       </c>
       <c r="G5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J5">
         <v>54</v>
@@ -1276,7 +1283,7 @@
         <v>667</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="J6">
         <v>74</v>
@@ -1322,7 +1329,7 @@
         <v>608</v>
       </c>
       <c r="G8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J8">
         <v>42</v>
@@ -1384,8 +1391,14 @@
       <c r="C11" t="s">
         <v>4</v>
       </c>
+      <c r="D11" s="2">
+        <v>43462</v>
+      </c>
       <c r="F11">
         <v>404</v>
+      </c>
+      <c r="G11">
+        <v>9</v>
       </c>
       <c r="J11">
         <v>28</v>
@@ -1464,8 +1477,14 @@
       <c r="C15" t="s">
         <v>4</v>
       </c>
+      <c r="D15" s="2">
+        <v>43456</v>
+      </c>
       <c r="F15">
         <v>270</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
       </c>
       <c r="J15">
         <v>31</v>
@@ -1488,7 +1507,7 @@
         <v>265</v>
       </c>
       <c r="G16">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="J16">
         <v>38</v>
@@ -1668,9 +1687,14 @@
       <c r="C25" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2">
+        <v>43470</v>
+      </c>
       <c r="F25">
         <v>112</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
       </c>
       <c r="H25" s="2">
         <v>43438</v>
@@ -1698,11 +1722,14 @@
       <c r="D26" s="2">
         <v>43417</v>
       </c>
+      <c r="E26" s="2">
+        <v>43470</v>
+      </c>
       <c r="F26">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="G26">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J26">
         <v>8</v>
@@ -1718,9 +1745,17 @@
       <c r="C27" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2">
+        <v>43462</v>
+      </c>
+      <c r="E27" s="2">
+        <v>43462</v>
+      </c>
       <c r="F27">
         <v>90</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
       </c>
       <c r="J27">
         <v>7</v>
@@ -1736,8 +1771,17 @@
       <c r="C28" t="s">
         <v>4</v>
       </c>
+      <c r="D28" s="2">
+        <v>43456</v>
+      </c>
+      <c r="E28" s="2">
+        <v>43461</v>
+      </c>
       <c r="F28">
         <v>87</v>
+      </c>
+      <c r="G28">
+        <v>4</v>
       </c>
       <c r="J28">
         <v>8</v>
@@ -1756,12 +1800,14 @@
       <c r="D29" s="2">
         <v>43427</v>
       </c>
-      <c r="E29" s="2"/>
+      <c r="E29" s="2">
+        <v>43455</v>
+      </c>
       <c r="F29">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J29">
         <v>3</v>
@@ -1777,8 +1823,17 @@
       <c r="C30" t="s">
         <v>4</v>
       </c>
+      <c r="D30" s="2">
+        <v>43454</v>
+      </c>
+      <c r="E30" s="2">
+        <v>43454</v>
+      </c>
       <c r="F30">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
       </c>
       <c r="J30">
         <v>1</v>
@@ -1794,9 +1849,17 @@
       <c r="C31" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="2"/>
+      <c r="D31" s="2">
+        <v>43454</v>
+      </c>
+      <c r="E31" s="2">
+        <v>43454</v>
+      </c>
       <c r="F31">
-        <v>61</v>
+        <v>63</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
       </c>
       <c r="J31">
         <v>4</v>
@@ -1812,8 +1875,17 @@
       <c r="C32" t="s">
         <v>4</v>
       </c>
+      <c r="D32" s="2">
+        <v>43454</v>
+      </c>
+      <c r="E32" s="2">
+        <v>43454</v>
+      </c>
       <c r="F32">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
       </c>
       <c r="J32">
         <v>5</v>
@@ -1836,7 +1908,7 @@
         <v>43438</v>
       </c>
       <c r="F33">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G33">
         <v>1</v>
@@ -3911,7 +3983,7 @@
         <v>4</v>
       </c>
       <c r="G95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H95" s="2">
         <v>43438</v>

</xml_diff>

<commit_message>
Updated lit review progress notes
</commit_message>
<xml_diff>
--- a/systematic lit review progress notes.xlsx
+++ b/systematic lit review progress notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherineschluth/bansallab/humanhelminths/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21C3B18F-91C7-7A41-AAFF-D51FE4D8F8F3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F932D885-7ACF-0E4E-B04A-73A31D461368}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1125,7 +1125,7 @@
   <dimension ref="A1:L233"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1190,7 +1190,7 @@
         <v>2319</v>
       </c>
       <c r="G2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J2">
         <v>237</v>
@@ -1259,7 +1259,7 @@
         <v>705</v>
       </c>
       <c r="G5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J5">
         <v>54</v>
@@ -1282,7 +1282,7 @@
         <v>667</v>
       </c>
       <c r="G6">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J6">
         <v>74</v>
@@ -1328,7 +1328,7 @@
         <v>608</v>
       </c>
       <c r="G8">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J8">
         <v>42</v>
@@ -1397,7 +1397,7 @@
         <v>404</v>
       </c>
       <c r="G11">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="J11">
         <v>28</v>

</xml_diff>